<commit_message>
decimal values with Paypal corrected
Fixed an error when calculating decimal values ​​with Paypal
</commit_message>
<xml_diff>
--- a/Teileliste.xlsx
+++ b/Teileliste.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\gesichert\github\honigautomat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF969EDA-DD02-4D59-AB91-8B68E9797BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD640E0-A28F-4507-8FB7-E15905495E4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31335" yWindow="1290" windowWidth="24945" windowHeight="21180" xr2:uid="{97770CAC-3B54-4B52-950E-CA345E4FEEE4}"/>
+    <workbookView xWindow="18915" yWindow="2430" windowWidth="30480" windowHeight="17700" xr2:uid="{97770CAC-3B54-4B52-950E-CA345E4FEEE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="92">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -233,9 +233,6 @@
     <t>https://www.ebay.de/itm/184891176473</t>
   </si>
   <si>
-    <t>Power On (12v / 16mm)</t>
-  </si>
-  <si>
     <t>Drucktaster (5v / 16 mm)</t>
   </si>
   <si>
@@ -339,6 +336,15 @@
   </si>
   <si>
     <t>https://www.az-delivery.de/pages/search-results-page?q=lcd%20display%2016x2%20i2c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keypad </t>
+  </si>
+  <si>
+    <t>bei Nutzung vom Keypad werden die externen Knöpfe nicht mehr genutzt - man benötigt also nur noch die internen (Prog &amp; Refill) sowie den externen Einschalttaster, sofern man Powersave nutzt</t>
+  </si>
+  <si>
+    <t>Power On (12v / 16mm) TASTER (nicht permanent)</t>
   </si>
 </sst>
 </file>
@@ -548,9 +554,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -559,6 +562,9 @@
     </xf>
     <xf numFmtId="8" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1354,6 +1360,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>762001</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>142170</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>105767</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Grafik 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9717091-D01A-D441-2AF8-B807C1622DF0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762001" y="30841950"/>
+          <a:ext cx="8190794" cy="4068167"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1657,10 +1707,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K83"/>
+  <dimension ref="A1:K114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1709,7 +1759,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C3" s="6">
         <v>1</v>
@@ -1731,7 +1781,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C4" s="6">
         <v>1</v>
@@ -1753,7 +1803,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C5" s="6">
         <v>1</v>
@@ -1775,7 +1825,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C6" s="6">
         <v>1</v>
@@ -1797,7 +1847,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C7" s="6">
         <v>1</v>
@@ -1819,7 +1869,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C8" s="6">
         <v>1</v>
@@ -1836,12 +1886,12 @@
       </c>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C9" s="6">
         <v>1</v>
@@ -1863,7 +1913,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C10" s="6">
         <v>1</v>
@@ -1882,10 +1932,10 @@
     </row>
     <row r="11" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C11" s="6">
         <v>5</v>
@@ -1904,7 +1954,7 @@
     </row>
     <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>54</v>
+        <v>91</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>53</v>
@@ -1982,7 +2032,7 @@
         <v>50</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G16" s="23">
         <v>2.79</v>
@@ -1990,7 +2040,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F17" s="23">
         <v>2</v>
@@ -2033,41 +2083,41 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="26"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
       <c r="E21" s="25"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
+      <c r="A22" s="26"/>
       <c r="B22" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="29">
+      <c r="D22" s="28">
         <v>3.53</v>
       </c>
       <c r="E22" s="25"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="27"/>
+      <c r="A23" s="26"/>
       <c r="B23" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="29"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="28"/>
       <c r="E23" s="25"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
+      <c r="A24" s="26"/>
       <c r="B24" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="28"/>
-      <c r="D24" s="29"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="28"/>
       <c r="E24" s="25"/>
       <c r="F24" s="23">
         <v>3.53</v>
@@ -2077,68 +2127,68 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="27"/>
+      <c r="A25" s="26"/>
       <c r="B25" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="28"/>
-      <c r="D25" s="29"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="28"/>
       <c r="E25" s="25"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="27"/>
+      <c r="A26" s="26"/>
       <c r="B26" s="11"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="29"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="28"/>
       <c r="E26" s="25"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="27"/>
+      <c r="A27" s="26"/>
       <c r="B27" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="28"/>
-      <c r="D27" s="29"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="28"/>
       <c r="E27" s="25"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="27"/>
+      <c r="A28" s="26"/>
       <c r="B28" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="28" t="s">
+      <c r="C28" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="D28" s="29">
+      <c r="D28" s="28">
         <v>6</v>
       </c>
       <c r="E28" s="25"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="27"/>
+      <c r="A29" s="26"/>
       <c r="B29" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="28"/>
-      <c r="D29" s="29"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="28"/>
       <c r="E29" s="25"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="27"/>
+      <c r="A30" s="26"/>
       <c r="B30" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="28"/>
-      <c r="D30" s="29"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="28"/>
       <c r="E30" s="25"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="27"/>
+      <c r="A31" s="26"/>
       <c r="B31" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="28"/>
-      <c r="D31" s="29"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="28"/>
       <c r="E31" s="25"/>
       <c r="F31" s="23">
         <v>6</v>
@@ -2148,43 +2198,43 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="27"/>
+      <c r="A32" s="26"/>
       <c r="B32" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C32" s="28"/>
-      <c r="D32" s="29"/>
+        <v>64</v>
+      </c>
+      <c r="C32" s="27"/>
+      <c r="D32" s="28"/>
       <c r="E32" s="25"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="27"/>
+      <c r="A33" s="26"/>
       <c r="B33" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="C33" s="28"/>
-      <c r="D33" s="29"/>
+        <v>63</v>
+      </c>
+      <c r="C33" s="27"/>
+      <c r="D33" s="28"/>
       <c r="E33" s="25"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="27"/>
+      <c r="A34" s="26"/>
       <c r="B34" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C34" s="28" t="s">
+      <c r="C34" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D34" s="29">
+      <c r="D34" s="28">
         <v>6.28</v>
       </c>
       <c r="E34" s="25"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="27"/>
+      <c r="A35" s="26"/>
       <c r="B35" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="28"/>
-      <c r="D35" s="29"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="28"/>
       <c r="E35" s="25"/>
       <c r="F35" s="23">
         <v>6.28</v>
@@ -2194,61 +2244,61 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="27"/>
+      <c r="A36" s="26"/>
       <c r="B36" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C36" s="28"/>
-      <c r="D36" s="29"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="28"/>
       <c r="E36" s="25"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="27"/>
+      <c r="A37" s="26"/>
       <c r="B37" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C37" s="28"/>
-      <c r="D37" s="29"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="28"/>
       <c r="E37" s="25"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="27"/>
+      <c r="A38" s="26"/>
       <c r="B38" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C38" s="28"/>
-      <c r="D38" s="29"/>
+        <v>65</v>
+      </c>
+      <c r="C38" s="27"/>
+      <c r="D38" s="28"/>
       <c r="E38" s="25"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="27"/>
+      <c r="A39" s="26"/>
       <c r="B39" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C39" s="28"/>
-      <c r="D39" s="29"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="28"/>
       <c r="E39" s="25"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="27"/>
+      <c r="A40" s="26"/>
       <c r="B40" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C40" s="28" t="s">
+      <c r="C40" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D40" s="29">
+      <c r="D40" s="28">
         <v>2.16</v>
       </c>
       <c r="E40" s="25"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="27"/>
+      <c r="A41" s="26"/>
       <c r="B41" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C41" s="28"/>
-      <c r="D41" s="29"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="28"/>
       <c r="E41" s="25"/>
       <c r="F41" s="23">
         <v>2.16</v>
@@ -2258,77 +2308,77 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="27"/>
+      <c r="A42" s="26"/>
       <c r="B42" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C42" s="28"/>
-      <c r="D42" s="29"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="28"/>
       <c r="E42" s="25"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="27"/>
+      <c r="A43" s="26"/>
       <c r="B43" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C43" s="28"/>
-      <c r="D43" s="29"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="28"/>
       <c r="E43" s="25"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="27"/>
+      <c r="A44" s="26"/>
       <c r="B44" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C44" s="27"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="25"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="26"/>
+      <c r="B45" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C44" s="28"/>
-      <c r="D44" s="29"/>
-      <c r="E44" s="25"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="27"/>
-      <c r="B45" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C45" s="28"/>
-      <c r="D45" s="29"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="28"/>
       <c r="E45" s="25"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="27"/>
+      <c r="A46" s="26"/>
       <c r="B46" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C46" s="28"/>
-      <c r="D46" s="29"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="28"/>
       <c r="E46" s="25"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="26"/>
-      <c r="B47" s="26"/>
-      <c r="C47" s="26"/>
-      <c r="D47" s="26"/>
+      <c r="A47" s="29"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="29"/>
+      <c r="D47" s="29"/>
       <c r="E47" s="25"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="27"/>
+      <c r="A48" s="26"/>
       <c r="B48" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C48" s="28" t="s">
+      <c r="C48" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D48" s="29">
+      <c r="D48" s="28">
         <v>4.34</v>
       </c>
       <c r="E48" s="25"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="27"/>
+      <c r="A49" s="26"/>
       <c r="B49" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C49" s="28"/>
-      <c r="D49" s="29"/>
+      <c r="C49" s="27"/>
+      <c r="D49" s="28"/>
       <c r="E49" s="25"/>
       <c r="F49" s="23">
         <v>4.34</v>
@@ -2338,44 +2388,44 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="27"/>
+      <c r="A50" s="26"/>
       <c r="B50" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C50" s="28"/>
-      <c r="D50" s="29"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="28"/>
       <c r="E50" s="25"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="27"/>
+      <c r="A51" s="26"/>
       <c r="B51" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C51" s="28"/>
-      <c r="D51" s="29"/>
+      <c r="C51" s="27"/>
+      <c r="D51" s="28"/>
       <c r="E51" s="25"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="27"/>
+      <c r="A52" s="26"/>
       <c r="B52" s="11"/>
-      <c r="C52" s="28"/>
-      <c r="D52" s="29"/>
+      <c r="C52" s="27"/>
+      <c r="D52" s="28"/>
       <c r="E52" s="25"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="27"/>
+      <c r="A53" s="26"/>
       <c r="B53" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C53" s="28"/>
-      <c r="D53" s="29"/>
+      <c r="C53" s="27"/>
+      <c r="D53" s="28"/>
       <c r="E53" s="25"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="26"/>
-      <c r="B54" s="26"/>
-      <c r="C54" s="26"/>
-      <c r="D54" s="26"/>
+      <c r="A54" s="29"/>
+      <c r="B54" s="29"/>
+      <c r="C54" s="29"/>
+      <c r="D54" s="29"/>
       <c r="E54" s="25"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -2411,7 +2461,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B61" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D61">
         <v>3.38</v>
@@ -2429,31 +2479,31 @@
     </row>
     <row r="64" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B64" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>71</v>
+      </c>
+      <c r="B66" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="B66" s="16" t="s">
+      <c r="C66" t="s">
         <v>73</v>
       </c>
-      <c r="C66" t="s">
+      <c r="D66" t="s">
         <v>74</v>
-      </c>
-      <c r="D66" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B69" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -2471,40 +2521,40 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B73" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B74" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B75" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B76" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B77" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B79" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B80" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D80" s="23">
         <v>9.49</v>
@@ -2512,7 +2562,7 @@
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B81" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D81" s="23">
         <v>25.99</v>
@@ -2520,7 +2570,7 @@
     </row>
     <row r="82" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B82" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D82" s="23">
         <v>39.9</v>
@@ -2528,7 +2578,7 @@
     </row>
     <row r="83" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B83" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D83" s="23">
         <v>5</v>
@@ -2538,8 +2588,28 @@
         <v>80.38</v>
       </c>
     </row>
+    <row r="114" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>89</v>
+      </c>
+      <c r="B114" s="16" t="s">
+        <v>90</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="E47:E54"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="A48:A53"/>
+    <mergeCell ref="C48:C53"/>
+    <mergeCell ref="D48:D53"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="E21:E27"/>
+    <mergeCell ref="E28:E33"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:A27"/>
+    <mergeCell ref="C22:C27"/>
+    <mergeCell ref="D22:D27"/>
     <mergeCell ref="E40:E46"/>
     <mergeCell ref="A28:A33"/>
     <mergeCell ref="C28:C33"/>
@@ -2551,18 +2621,6 @@
     <mergeCell ref="A40:A46"/>
     <mergeCell ref="C40:C46"/>
     <mergeCell ref="D40:D46"/>
-    <mergeCell ref="E21:E27"/>
-    <mergeCell ref="E28:E33"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:A27"/>
-    <mergeCell ref="C22:C27"/>
-    <mergeCell ref="D22:D27"/>
-    <mergeCell ref="E47:E54"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="A48:A53"/>
-    <mergeCell ref="C48:C53"/>
-    <mergeCell ref="D48:D53"/>
-    <mergeCell ref="A54:D54"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{F70DF216-BE85-4716-BA3D-3B01FC614819}"/>

</xml_diff>